<commit_message>
Added a timeline for my course
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Digi Safari\Documents\Learning\JavaScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4815B6A1-ECDE-4B9A-B1CA-A17DD936B9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6771F-9D42-4FB9-9470-9A29E9AEB985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -36,30 +36,18 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Week 2</t>
   </si>
   <si>
     <t>Fundaments of JavaScript</t>
   </si>
   <si>
-    <t>Fundaments are completed</t>
-  </si>
-  <si>
     <t>Fundaments of JavaScript (ES6 Onwards)</t>
   </si>
   <si>
-    <t>Preparing for ES6 changes</t>
-  </si>
-  <si>
     <t>Structured Data Types(Arrays, Tree, Matrix)</t>
   </si>
   <si>
-    <t>Assignements</t>
-  </si>
-  <si>
     <t>OOPS in JavaScript(Stacks, Queue, Linked-List)</t>
   </si>
   <si>
@@ -85,6 +73,42 @@
   </si>
   <si>
     <t>Off-Track</t>
+  </si>
+  <si>
+    <t>HTML, CSS and JavaScript Crash Course</t>
+  </si>
+  <si>
+    <t>Not-Started</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>DOM Events</t>
+  </si>
+  <si>
+    <t>Mordern JavaScript Tools</t>
   </si>
 </sst>
 </file>
@@ -92,8 +116,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -193,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -203,16 +227,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -220,9 +244,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -234,7 +256,22 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -244,52 +281,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -572,178 +626,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69" style="15" customWidth="1"/>
+    <col min="4" max="4" width="16" style="15" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="7" width="14.28515625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10">
+        <v>45635</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10">
+        <v>45636</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="10">
+        <v>45637</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="10">
+        <v>45638</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="10">
+        <v>45639</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="10">
+        <v>45640</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="10">
+        <v>45641</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
-        <v>45635</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
-        <v>45636</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="2" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
-        <v>45637</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="B13" s="10">
+        <v>45642</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10">
+        <v>45643</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
-        <v>45638</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10">
+        <v>45644</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
-        <v>45639</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
-        <v>45642</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
-        <v>45643</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
-        <v>45644</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>45645</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="D15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>